<commit_message>
now new excel file updates automatically
</commit_message>
<xml_diff>
--- a/streamlit/housesTRIAL.xlsx
+++ b/streamlit/housesTRIAL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E855"/>
+  <dimension ref="A1:E854"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>120 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>57</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,24 +478,24 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Debrecen, Sinai Miklós</t>
+          <t>Debrecen , Böszörményi street</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-sinai-miklos-utca-1-bedroom-living-room-apartament-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/furedi-residential-area-flat-for-rent-2/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>120 000</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,159 +505,159 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Debrecen, Kardos Albert</t>
+          <t>Debrecen, Sinai Miklós</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-kardos-albert-street-2-separate-rooms-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-sinai-miklos-utca-1-bedroom-living-room-apartament-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>280 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>59</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1 living room(s), 4 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Debrecen, Komlóssy street</t>
+          <t>Debrecen, Kardos Albert</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen1-min-from-the-uni-main-4-bedroom-living-room-apartment-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-kardos-albert-street-2-separate-rooms-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>420 000</t>
+          <t>280 000</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 4 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Debrecen, Rákóczi</t>
+          <t>Debrecen, Komlóssy street</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-belvaros-3-bedroom-living-room-unfurnished-apartament-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen1-min-from-the-uni-main-4-bedroom-living-room-apartment-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>180 000</t>
+          <t>420 000</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>112</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Debrecen, Mikszáth Kálmán street</t>
+          <t>Debrecen, Rákóczi</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/mikszath-kalman-street-close-to-uni-2-rooms-flat-available/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-belvaros-3-bedroom-living-room-unfurnished-apartament-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>760 000</t>
+          <t>180 000</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 0  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Debrecen, Pacsirta</t>
+          <t>Debrecen, Mikszáth Kálmán street</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-house-for-rent-3-bedroom-living-room/</t>
+          <t>https://www.findahome.hu/ingatlanok/mikszath-kalman-street-close-to-uni-2-rooms-flat-available/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>120 000</t>
+          <t>760 000</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 0  bathroom(s)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Debrecen, Domokos Lajos</t>
+          <t>Debrecen, Pacsirta</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-domokos-lajos-street-1-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-house-for-rent-3-bedroom-living-room/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>200 000</t>
+          <t>120 000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -667,12 +667,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Debrecen , Böszörményi street</t>
+          <t>Debrecen, Domokos Lajos</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/furedi-residential-area-flat-for-rent-2/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-domokos-lajos-street-1-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -922,54 +922,54 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>250 000</t>
+          <t>67 900 000</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>98</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1 living room(s), 4 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Debrecen, Péchy</t>
+          <t>Debrecen, Vasútoldal</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/4-bedroom-living-room-house-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/elado-csaladi-haz-feszek-lakoparkban/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>250 000</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 4 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Debrecen, Sánta Kálmán</t>
+          <t>Debrecen, Péchy</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-santa-kalman-street-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/4-bedroom-living-room-house-for-rent/</t>
         </is>
       </c>
     </row>
@@ -981,34 +981,34 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Debrecen, Bajcsy Zsilinszky</t>
+          <t>Debrecen, Sánta Kálmán</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/city-center-bajcsy-zsilinszky-street-2-spacious-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-santa-kalman-street-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>165 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>75</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1018,19 +1018,19 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Debrecen, Apafi</t>
+          <t>Debrecen, Bajcsy Zsilinszky</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-apafi-street-close-to-the-kassai-campus-1-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/city-center-bajcsy-zsilinszky-street-2-spacious-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>175 000</t>
+          <t>165 000</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1045,267 +1045,267 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Debrecen, Honvéd street</t>
+          <t>Debrecen, Apafi</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/cozy-flat-for-rent-close-to-the-city-center/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-apafi-street-close-to-the-kassai-campus-1-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>175 000</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Debrecen, Böszörményi street</t>
+          <t>Debrecen, Honvéd street</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/boszormenyi-street-3-separate-room-dining-area-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/cozy-flat-for-rent-close-to-the-city-center/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>200 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>64</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Debrecen , Kassai street</t>
+          <t>Debrecen, Böszörményi street</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/3-bedrooms-livng-room-flat-for-rent-close-to-kassai-campus/</t>
+          <t>https://www.findahome.hu/ingatlanok/boszormenyi-street-3-separate-room-dining-area-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>200 000</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>80</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Debrecen, Görgey street</t>
+          <t>Debrecen , Kassai street</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/gorgey-street-near-uni-2-rooms-flat-availabe-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/3-bedrooms-livng-room-flat-for-rent-close-to-kassai-campus/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>40 900 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Debrecen, Egyetem sugárút</t>
+          <t>Debrecen, Görgey street</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/egyetem-sgt-renovated-modern-2-rooms-flat-ideal-2-3-person-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/gorgey-street-near-uni-2-rooms-flat-availabe-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>480 000</t>
+          <t>40 900 000</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Debrecen, Garai</t>
+          <t>Debrecen, Egyetem sugárút</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-brand-new-2-bedroom-living-room-apartment-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/egyetem-sgt-renovated-modern-2-rooms-flat-ideal-2-3-person-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>110 000</t>
+          <t>480 000</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Debrecen, Bólyai</t>
+          <t>Debrecen, Garai</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/lakas-kiado-a-bolyai-utcan/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-brand-new-2-bedroom-living-room-apartment-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>450 000</t>
+          <t>110 000</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Debrecen, Fészek lakópark</t>
+          <t>Debrecen, Bólyai</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-feszek-lakopark-3-bedroom-living-room-house-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/lakas-kiado-a-bolyai-utcan/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>37 600 000</t>
+          <t>450 000</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>175</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Debrecen, István</t>
+          <t>Debrecen, Fészek lakópark</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/istvan-uton-lakas-elado/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-feszek-lakopark-3-bedroom-living-room-house-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>300 000</t>
+          <t>37 600 000</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Debrecen, Párizsi udvar</t>
+          <t>Debrecen, István</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-parizsi-udvar-3-room-70-sqm-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/istvan-uton-lakas-elado/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>200 000</t>
+          <t>300 000</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>70</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1315,240 +1315,240 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvani István</t>
+          <t>Debrecen, Párizsi udvar</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-3-rooms-ac-new-building-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-parizsi-udvar-3-room-70-sqm-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>200 000</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Debrecen, Viola</t>
+          <t>Debrecen, Hatvani István</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-viola-street-1-bedroom-living-room-flat-fo-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-3-rooms-ac-new-building-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>125 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1 living room(s), 0 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Debrecen, Budai Nagy Antal</t>
+          <t>Debrecen, Viola</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/kiado-haz-a-budai-nagy-antal-utcan/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-viola-street-1-bedroom-living-room-flat-fo-rent/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>235 000</t>
+          <t>125 000</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 0 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Debrecen, Dessewffy</t>
+          <t>Debrecen, Budai Nagy Antal</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-a-belvaros-kozeleben/</t>
+          <t>https://www.findahome.hu/ingatlanok/kiado-haz-a-budai-nagy-antal-utcan/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>250 000</t>
+          <t>235 000</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>43</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Debrecen, Arany jános</t>
+          <t>Debrecen, Dessewffy</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/city-center-3-separate-room-fully-furnsihed-and-equipped-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-a-belvaros-kozeleben/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>130 000</t>
+          <t>250 000</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>72</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Debrecen, Jerikó</t>
+          <t>Debrecen, Arany jános</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-jeriko-utcan/</t>
+          <t>https://www.findahome.hu/ingatlanok/city-center-3-separate-room-fully-furnsihed-and-equipped-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>15 000 000</t>
+          <t>130 000</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>44</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Debrecen, Virágpor</t>
+          <t>Debrecen, Jerikó</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/elado-haz-gaspar-gyorgy-kert/</t>
+          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-jeriko-utcan/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>29 500 000</t>
+          <t>15 000 000</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Debrecen, Ókút</t>
+          <t>Debrecen, Virágpor</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/elado-lakas-az-egyetem-sugarut-kozeleben/</t>
+          <t>https://www.findahome.hu/ingatlanok/elado-haz-gaspar-gyorgy-kert/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>43 000 000</t>
+          <t>29 500 000</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Debrecen, Kocsis</t>
+          <t>Debrecen, Ókút</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/elado-kertes-haz-alkalmi-aron/</t>
+          <t>https://www.findahome.hu/ingatlanok/elado-lakas-az-egyetem-sugarut-kozeleben/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>43 000 000</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>65</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1558,24 +1558,24 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó</t>
+          <t>Debrecen, Kocsis</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-csapo-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/elado-kertes-haz-alkalmi-aron/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>280 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>61</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1585,24 +1585,24 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Debrecen, Rákóczi</t>
+          <t>Debrecen, Csapó</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-rakoczi-utca/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-csapo-street/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>410 000</t>
+          <t>280 000</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>68</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1612,56 +1612,56 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Debrecen, Piac</t>
+          <t>Debrecen, Rákóczi</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-piac-street-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-rakoczi-utca/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>180 000</t>
+          <t>410 000</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>106</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Debrecen, Böszörményi</t>
+          <t>Debrecen, Piac</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-furedi-lakopark/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-piac-street-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>265 000</t>
+          <t>180 000</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1671,73 +1671,73 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-boszormenyi-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-furedi-lakopark/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>55 000</t>
+          <t>265 000</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>58</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Debrecen, Jerikó</t>
+          <t>Debrecen, Böszörményi</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-jeriko-street-only-room-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-boszormenyi-street/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>130 000</t>
+          <t>55 000</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvani István</t>
+          <t>Debrecen, Jerikó</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-1-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-jeriko-street-only-room-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>145 000</t>
+          <t>130 000</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1747,159 +1747,159 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Debrecen, Dózsa György</t>
+          <t>Debrecen, Hatvani István</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-venkert/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-1-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>145 000</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Debrecen, Báthori</t>
+          <t>Debrecen, Dózsa György</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/kiado-csaladi-haz-a-bathori-utcan/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-venkert/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>175 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1 living room(s), 0 bedroom(s), 2  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Debrecen, Kétmalom</t>
+          <t>Debrecen, Báthori</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-ketmalom-utca/</t>
+          <t>https://www.findahome.hu/ingatlanok/kiado-csaladi-haz-a-bathori-utcan/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>175 000</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>70</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 0 bedroom(s), 2  bathroom(s)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>, Ispotály</t>
+          <t>Debrecen, Kétmalom</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-az-ispotaly-utcan/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-ketmalom-utca/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>275 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvan utcai kert</t>
+          <t>, Ispotály</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-hatvan-utcai-kert/</t>
+          <t>https://www.findahome.hu/ingatlanok/kiado-lakas-az-ispotaly-utcan/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>275 000</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>80</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Debrecen, Poroszlay</t>
+          <t>Debrecen, Hatvan utcai kert</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-poroszlay-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-hatvan-utcai-kert/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>120 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>62</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1909,19 +1909,19 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Debrecen, Hadházi</t>
+          <t>Debrecen, Poroszlay</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-hadhazi-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-poroszlay-street/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>160 000</t>
+          <t>120 000</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1936,186 +1936,186 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Debrecen, Teleki</t>
+          <t>Debrecen, Hadházi</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-teleki-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-hadhazi-street/</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>220 000</t>
+          <t>160 000</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Debrecen, Bethlen</t>
+          <t>Debrecen, Teleki</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-the-city-center/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-teleki-street/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>145 000</t>
+          <t>220 000</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Debrecen, Klaipeda</t>
+          <t>Debrecen, Bethlen</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-on-klaipeda-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-the-city-center/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>34 900 000</t>
+          <t>145 000</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>58</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Debrecen, Füredi</t>
+          <t>Debrecen, Klaipeda</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/elado-lakas-a-furedi-uton/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-on-klaipeda-street/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>185 000</t>
+          <t>34 900 000</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Debrecen, Nap</t>
+          <t>Debrecen, Füredi</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-on-nap-utca/</t>
+          <t>https://www.findahome.hu/ingatlanok/elado-lakas-a-furedi-uton/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>185 000</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>42</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 0  bathroom(s)</t>
+          <t>1 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Debrecen, Darabos</t>
+          <t>Debrecen, Nap</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-1-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-on-nap-utca/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>250 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>44</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 0  bathroom(s)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Debrecen, Simonffy</t>
+          <t>Debrecen, Darabos</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-simonffy-street-3-bedroom-living-oom-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-1-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>600 000</t>
+          <t>250 000</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2125,29 +2125,29 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Debrecen, Bajcsy-Zsilinszky</t>
+          <t>Debrecen, Simonffy</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-simonffy-street-3-bedroom-living-oom-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>600 000</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>93</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2 living room(s), 0 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/office-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent/</t>
         </is>
       </c>
     </row>
@@ -2169,34 +2169,34 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>75</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>2 living room(s), 0 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Debrecen, Derék</t>
+          <t>Debrecen, Bajcsy-Zsilinszky</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-tocovolgy/</t>
+          <t>https://www.findahome.hu/ingatlanok/office-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>160 000</t>
+          <t>150 000</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>63</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2206,51 +2206,51 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Debrecen, Zöldfa</t>
+          <t>Debrecen, Derék</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/zoldfa-utcan-butorozatlan-lakas-kiado/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-in-tocovolgy/</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>110 000</t>
+          <t>160 000</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>73</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
+          <t>1 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Debrecen, Karácsony György</t>
+          <t>Debrecen, Zöldfa</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-on-karacsony-gyorgy-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/zoldfa-utcan-butorozatlan-lakas-kiado/</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>120 000</t>
+          <t>110 000</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2260,66 +2260,66 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Debrecen, Mata János</t>
+          <t>Debrecen, Karácsony György</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-mata-janos-utca/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-on-karacsony-gyorgy-street/</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>130 000</t>
+          <t>120 000</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 2 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Debrecen, Halköz</t>
+          <t>Debrecen, Mata János</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/in-the-middle-of-the-city-center-modern-studio-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-mata-janos-utca/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>69 900 000</t>
+          <t>130 000</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1 living room(s), 3 bedroom(s), 1  bathroom(s)</t>
+          <t>0 living room(s), 1 bedroom(s), 1  bathroom(s)</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Debrecen, Vasútoldal</t>
+          <t>Debrecen, Halköz</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/elado-csaladi-haz-feszek-lakoparkban/</t>
+          <t>https://www.findahome.hu/ingatlanok/in-the-middle-of-the-city-center-modern-studio-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -19462,35 +19462,31 @@
     <row r="723">
       <c r="A723" t="inlineStr">
         <is>
-          <t>270 000</t>
+          <t>400 000</t>
         </is>
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>72</t>
-        </is>
-      </c>
-      <c r="C723" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>214</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr"/>
       <c r="D723" t="inlineStr"/>
       <c r="E723" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99593-debrecen-flat</t>
+          <t>https://www.greatforest.hu/property/98597-debrecen-eastern-western-industrial-area-industrial-building</t>
         </is>
       </c>
     </row>
     <row r="724">
       <c r="A724" t="inlineStr">
         <is>
-          <t>280 000</t>
+          <t>200 000</t>
         </is>
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C724" t="inlineStr">
@@ -19501,168 +19497,168 @@
       <c r="D724" t="inlineStr"/>
       <c r="E724" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99590-debrecen-flat</t>
+          <t>https://www.greatforest.hu/property/20816-debrecen-city-north-part-of-a-house</t>
         </is>
       </c>
     </row>
     <row r="725">
       <c r="A725" t="inlineStr">
         <is>
-          <t>230 000</t>
+          <t>375 000</t>
         </is>
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>82</t>
         </is>
       </c>
       <c r="C725" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D725" t="inlineStr"/>
       <c r="E725" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99587-debrecen-flat</t>
+          <t>https://www.greatforest.hu/property/96519-debrecen-greatforest-area-flat</t>
         </is>
       </c>
     </row>
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>250 000</t>
+          <t>490 000</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>288</t>
         </is>
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D726" t="inlineStr"/>
       <c r="E726" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99332-debrecen-bem-square-office-in-office-building</t>
+          <t>https://www.greatforest.hu/property/100132-debrecen-close-to-bem-square-family-house</t>
         </is>
       </c>
     </row>
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>220 000</t>
+          <t>290 000</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D727" t="inlineStr"/>
       <c r="E727" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99213-debrecen-close-to-main-campus-flat</t>
+          <t>https://www.greatforest.hu/property/65827-debrecen-close-to-bem-square-part-of-a-house</t>
         </is>
       </c>
     </row>
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>350 000</t>
+          <t>130 000</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D728" t="inlineStr"/>
       <c r="E728" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/89979-debrecen-city-center-office-not-in-office-building</t>
+          <t>https://www.greatforest.hu/property/84773-debrecen-close-to-plaza-office-not-in-office-building</t>
         </is>
       </c>
     </row>
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>595 000</t>
+          <t>300 000</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>73</t>
         </is>
       </c>
       <c r="C729" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D729" t="inlineStr"/>
       <c r="E729" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/36059-debrecen-kassai-campus-area-flat</t>
+          <t>https://www.greatforest.hu/property/99598-debrecen-flat</t>
         </is>
       </c>
     </row>
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>300 000</t>
+          <t>230 000</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>64</t>
         </is>
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D730" t="inlineStr"/>
       <c r="E730" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/69432-debrecen-greatforest-area-flat</t>
+          <t>https://www.greatforest.hu/property/99597-debrecen-flat</t>
         </is>
       </c>
     </row>
     <row r="731">
       <c r="A731" t="inlineStr">
         <is>
-          <t>150 000</t>
+          <t>280 000</t>
         </is>
       </c>
       <c r="B731" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>88</t>
         </is>
       </c>
       <c r="C731" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D731" t="inlineStr"/>
       <c r="E731" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/65443-debrecen-city-west-office-in-office-building</t>
+          <t>https://www.greatforest.hu/property/99595-debrecen-flat</t>
         </is>
       </c>
     </row>
@@ -21165,12 +21161,12 @@
     <row r="808">
       <c r="A808" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B808" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>38</t>
         </is>
       </c>
       <c r="C808" t="inlineStr">
@@ -21180,78 +21176,78 @@
       </c>
       <c r="D808" t="inlineStr">
         <is>
-          <t>Debrecen, Görgey utca</t>
+          <t>Debrecen, Batthyány utca</t>
         </is>
       </c>
       <c r="E808" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gorgey-utca/219854/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-batthyany-utca/219726/</t>
         </is>
       </c>
     </row>
     <row r="809">
       <c r="A809" t="inlineStr">
         <is>
-          <t>160 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B809" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>0 Bedrooms, 1 Bathrooms</t>
+          <t>1 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D809" t="inlineStr">
         <is>
-          <t>Debrecen, Bem tér</t>
+          <t>Debrecen, Görgey utca</t>
         </is>
       </c>
       <c r="E809" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/207975/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gorgey-utca/219854/</t>
         </is>
       </c>
     </row>
     <row r="810">
       <c r="A810" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>160 000</t>
         </is>
       </c>
       <c r="B810" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>70</t>
         </is>
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>1 Bedrooms, 1 Bathrooms</t>
+          <t>0 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D810" t="inlineStr">
         <is>
-          <t>Debrecen, Cívis utca</t>
+          <t>Debrecen, Bem tér</t>
         </is>
       </c>
       <c r="E810" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-civis-utca/219199/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/207975/</t>
         </is>
       </c>
     </row>
     <row r="811">
       <c r="A811" t="inlineStr">
         <is>
-          <t>220 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B811" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C811" t="inlineStr">
@@ -21261,24 +21257,24 @@
       </c>
       <c r="D811" t="inlineStr">
         <is>
-          <t>Debrecen, Rózsahegy utca</t>
+          <t>Debrecen, Cívis utca</t>
         </is>
       </c>
       <c r="E811" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-rozsahegy-utca/209110/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-civis-utca/219199/</t>
         </is>
       </c>
     </row>
     <row r="812">
       <c r="A812" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>220 000</t>
         </is>
       </c>
       <c r="B812" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C812" t="inlineStr">
@@ -21288,24 +21284,24 @@
       </c>
       <c r="D812" t="inlineStr">
         <is>
-          <t>Debrecen, Széchenyi utca</t>
+          <t>Debrecen, Rózsahegy utca</t>
         </is>
       </c>
       <c r="E812" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szechenyi-utca/219233/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-rozsahegy-utca/209110/</t>
         </is>
       </c>
     </row>
     <row r="813">
       <c r="A813" t="inlineStr">
         <is>
-          <t>180 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B813" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C813" t="inlineStr">
@@ -21315,24 +21311,24 @@
       </c>
       <c r="D813" t="inlineStr">
         <is>
-          <t>Debrecen, Nagyerdei körút</t>
+          <t>Debrecen, Széchenyi utca</t>
         </is>
       </c>
       <c r="E813" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagyerdei-korut/199999/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szechenyi-utca/219233/</t>
         </is>
       </c>
     </row>
     <row r="814">
       <c r="A814" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>180 000</t>
         </is>
       </c>
       <c r="B814" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C814" t="inlineStr">
@@ -21342,24 +21338,24 @@
       </c>
       <c r="D814" t="inlineStr">
         <is>
-          <t>Debrecen, Kossuth utca</t>
+          <t>Debrecen, Nagyerdei körút</t>
         </is>
       </c>
       <c r="E814" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-kossuth-utca/219810/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagyerdei-korut/199999/</t>
         </is>
       </c>
     </row>
     <row r="815">
       <c r="A815" t="inlineStr">
         <is>
-          <t>185 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B815" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>41</t>
         </is>
       </c>
       <c r="C815" t="inlineStr">
@@ -21369,24 +21365,24 @@
       </c>
       <c r="D815" t="inlineStr">
         <is>
-          <t>Debrecen, Görgey utca</t>
+          <t>Debrecen, Kossuth utca</t>
         </is>
       </c>
       <c r="E815" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gorgey-utca/219815/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-kossuth-utca/219810/</t>
         </is>
       </c>
     </row>
     <row r="816">
       <c r="A816" t="inlineStr">
         <is>
-          <t>120 000</t>
+          <t>185 000</t>
         </is>
       </c>
       <c r="B816" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C816" t="inlineStr">
@@ -21396,24 +21392,24 @@
       </c>
       <c r="D816" t="inlineStr">
         <is>
-          <t>Debrecen, Vezér utca</t>
+          <t>Debrecen, Görgey utca</t>
         </is>
       </c>
       <c r="E816" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-vezer-utca/219797/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gorgey-utca/219815/</t>
         </is>
       </c>
     </row>
     <row r="817">
       <c r="A817" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>120 000</t>
         </is>
       </c>
       <c r="B817" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C817" t="inlineStr">
@@ -21423,105 +21419,105 @@
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>Debrecen, Bem tér</t>
+          <t>Debrecen, Vezér utca</t>
         </is>
       </c>
       <c r="E817" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/169681/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-vezer-utca/219797/</t>
         </is>
       </c>
     </row>
     <row r="818">
       <c r="A818" t="inlineStr">
         <is>
-          <t>280 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B818" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>3 Bedrooms, 1 Bathrooms</t>
+          <t>1 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D818" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó utca</t>
+          <t>Debrecen, Bem tér</t>
         </is>
       </c>
       <c r="E818" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/206077/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/169681/</t>
         </is>
       </c>
     </row>
     <row r="819">
       <c r="A819" t="inlineStr">
         <is>
-          <t>270 000</t>
+          <t>280 000</t>
         </is>
       </c>
       <c r="B819" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>92</t>
         </is>
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>3 Bedrooms, 2 Bathrooms</t>
+          <t>3 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D819" t="inlineStr">
         <is>
-          <t>Debrecen, Bartók Béla út</t>
+          <t>Debrecen, Csapó utca</t>
         </is>
       </c>
       <c r="E819" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/debrecen-bartok-bela-ut/163569/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/206077/</t>
         </is>
       </c>
     </row>
     <row r="820">
       <c r="A820" t="inlineStr">
         <is>
-          <t>119 000</t>
+          <t>270 000</t>
         </is>
       </c>
       <c r="B820" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>1 Bedrooms, 1 Bathrooms</t>
+          <t>3 Bedrooms, 2 Bathrooms</t>
         </is>
       </c>
       <c r="D820" t="inlineStr">
         <is>
-          <t>Debrecen, Kassai út</t>
+          <t>Debrecen, Bartók Béla út</t>
         </is>
       </c>
       <c r="E820" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/debrecen-kassai-ut/176619/</t>
+          <t>https://debrecenrent.hu/for-rent/house/debrecen-bartok-bela-ut/163569/</t>
         </is>
       </c>
     </row>
     <row r="821">
       <c r="A821" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>119 000</t>
         </is>
       </c>
       <c r="B821" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C821" t="inlineStr">
@@ -21531,24 +21527,24 @@
       </c>
       <c r="D821" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó utca</t>
+          <t>Debrecen, Kassai út</t>
         </is>
       </c>
       <c r="E821" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/212757/</t>
+          <t>https://debrecenrent.hu/for-rent/house/debrecen-kassai-ut/176619/</t>
         </is>
       </c>
     </row>
     <row r="822">
       <c r="A822" t="inlineStr">
         <is>
-          <t>115 000</t>
+          <t>140 000</t>
         </is>
       </c>
       <c r="B822" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C822" t="inlineStr">
@@ -21558,24 +21554,24 @@
       </c>
       <c r="D822" t="inlineStr">
         <is>
-          <t>Debrecen, Faraktár utca</t>
+          <t>Debrecen, Csapó utca</t>
         </is>
       </c>
       <c r="E822" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-faraktar-utca/219628/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/212757/</t>
         </is>
       </c>
     </row>
     <row r="823">
       <c r="A823" t="inlineStr">
         <is>
-          <t>490 000</t>
+          <t>115 000</t>
         </is>
       </c>
       <c r="B823" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C823" t="inlineStr">
@@ -21585,56 +21581,56 @@
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>Debrecen, Mikszáth Kálmán utca</t>
+          <t>Debrecen, Faraktár utca</t>
         </is>
       </c>
       <c r="E823" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-mikszath-kalman-utca/216981/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-faraktar-utca/219628/</t>
         </is>
       </c>
     </row>
     <row r="824">
       <c r="A824" t="inlineStr">
         <is>
-          <t>280 000</t>
+          <t>490 000</t>
         </is>
       </c>
       <c r="B824" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>2 Bedrooms, 1 Bathrooms</t>
+          <t>1 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D824" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó utca</t>
+          <t>Debrecen, Mikszáth Kálmán utca</t>
         </is>
       </c>
       <c r="E824" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/218738/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-mikszath-kalman-utca/216981/</t>
         </is>
       </c>
     </row>
     <row r="825">
       <c r="A825" t="inlineStr">
         <is>
-          <t>390 000</t>
+          <t>280 000</t>
         </is>
       </c>
       <c r="B825" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>68</t>
         </is>
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>3 Bedrooms, 1 Bathrooms</t>
+          <t>2 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D825" t="inlineStr">
@@ -21644,34 +21640,34 @@
       </c>
       <c r="E825" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/219320/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/218738/</t>
         </is>
       </c>
     </row>
     <row r="826">
       <c r="A826" t="inlineStr">
         <is>
-          <t>140 000</t>
+          <t>390 000</t>
         </is>
       </c>
       <c r="B826" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>115</t>
         </is>
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>1 Bedrooms, 1 Bathrooms</t>
+          <t>3 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D826" t="inlineStr">
         <is>
-          <t>Debrecen, Batthyány utca</t>
+          <t>Debrecen, Csapó utca</t>
         </is>
       </c>
       <c r="E826" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-batthyany-utca/219726/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/219320/</t>
         </is>
       </c>
     </row>
@@ -22083,12 +22079,12 @@
     <row r="842">
       <c r="A842" t="inlineStr">
         <is>
-          <t>130 000</t>
+          <t>240 000</t>
         </is>
       </c>
       <c r="B842" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C842" t="inlineStr">
@@ -22098,78 +22094,78 @@
       </c>
       <c r="D842" t="inlineStr">
         <is>
-          <t>Debrecen, Honvéd utca</t>
+          <t>Debrecen, Nagy Lajos király tér</t>
         </is>
       </c>
       <c r="E842" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-honved-utca/192083/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagy-lajos-kiraly-ter/218134/</t>
         </is>
       </c>
     </row>
     <row r="843">
       <c r="A843" t="inlineStr">
         <is>
-          <t>240 000</t>
+          <t>350 000</t>
         </is>
       </c>
       <c r="B843" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>1 Bedrooms, 1 Bathrooms</t>
+          <t>4 Bedrooms, 2 Bathrooms</t>
         </is>
       </c>
       <c r="D843" t="inlineStr">
         <is>
-          <t>Debrecen, Nagy Lajos király tér</t>
+          <t>Debrecen, Akadémia utca</t>
         </is>
       </c>
       <c r="E843" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagy-lajos-kiraly-ter/218134/</t>
+          <t>https://debrecenrent.hu/for-rent/house/debrecen-akademia-utca/217736/</t>
         </is>
       </c>
     </row>
     <row r="844">
       <c r="A844" t="inlineStr">
         <is>
-          <t>350 000</t>
+          <t>190 000</t>
         </is>
       </c>
       <c r="B844" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>65</t>
         </is>
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>4 Bedrooms, 2 Bathrooms</t>
+          <t>1 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D844" t="inlineStr">
         <is>
-          <t>Debrecen, Akadémia utca</t>
+          <t>Debrecen, Szoboszlói út</t>
         </is>
       </c>
       <c r="E844" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/debrecen-akademia-utca/217736/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szoboszloi-ut/204247/</t>
         </is>
       </c>
     </row>
     <row r="845">
       <c r="A845" t="inlineStr">
         <is>
-          <t>190 000</t>
+          <t>200 000</t>
         </is>
       </c>
       <c r="B845" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C845" t="inlineStr">
@@ -22179,24 +22175,24 @@
       </c>
       <c r="D845" t="inlineStr">
         <is>
-          <t>Debrecen, Szoboszlói út</t>
+          <t>Debrecen, Péterfia utca</t>
         </is>
       </c>
       <c r="E845" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szoboszloi-ut/204247/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/210104/</t>
         </is>
       </c>
     </row>
     <row r="846">
       <c r="A846" t="inlineStr">
         <is>
-          <t>200 000</t>
+          <t>170 000</t>
         </is>
       </c>
       <c r="B846" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C846" t="inlineStr">
@@ -22211,19 +22207,19 @@
       </c>
       <c r="E846" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/210104/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/215070/</t>
         </is>
       </c>
     </row>
     <row r="847">
       <c r="A847" t="inlineStr">
         <is>
-          <t>170 000</t>
+          <t>190 000</t>
         </is>
       </c>
       <c r="B847" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C847" t="inlineStr">
@@ -22238,7 +22234,7 @@
       </c>
       <c r="E847" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/215070/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/205429/</t>
         </is>
       </c>
     </row>
@@ -22250,7 +22246,7 @@
       </c>
       <c r="B848" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C848" t="inlineStr">
@@ -22265,19 +22261,19 @@
       </c>
       <c r="E848" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/205429/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/205422/</t>
         </is>
       </c>
     </row>
     <row r="849">
       <c r="A849" t="inlineStr">
         <is>
-          <t>190 000</t>
+          <t>230 000</t>
         </is>
       </c>
       <c r="B849" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C849" t="inlineStr">
@@ -22287,152 +22283,125 @@
       </c>
       <c r="D849" t="inlineStr">
         <is>
-          <t>Debrecen, Péterfia utca</t>
+          <t>Debrecen, Gönczy Pál utca</t>
         </is>
       </c>
       <c r="E849" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-peterfia-utca/205422/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gonczy-pal-utca/216064/</t>
         </is>
       </c>
     </row>
     <row r="850">
       <c r="A850" t="inlineStr">
         <is>
-          <t>230 000</t>
-        </is>
-      </c>
-      <c r="B850" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="C850" t="inlineStr">
-        <is>
-          <t>1 Bedrooms, 1 Bathrooms</t>
-        </is>
-      </c>
+          <t>600 000</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr"/>
+      <c r="C850" t="inlineStr"/>
       <c r="D850" t="inlineStr">
         <is>
-          <t>Debrecen, Gönczy Pál utca</t>
+          <t>Hajdúszoboszló</t>
         </is>
       </c>
       <c r="E850" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gonczy-pal-utca/216064/</t>
+          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-/214748/</t>
         </is>
       </c>
     </row>
     <row r="851">
       <c r="A851" t="inlineStr">
         <is>
-          <t>600 000</t>
-        </is>
-      </c>
-      <c r="B851" t="inlineStr"/>
-      <c r="C851" t="inlineStr"/>
+          <t>500 000</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>3 Bedrooms, 2 Bathrooms</t>
+        </is>
+      </c>
       <c r="D851" t="inlineStr">
         <is>
-          <t>Hajdúszoboszló</t>
+          <t>Hajdúszoboszló, Hőforrás utca</t>
         </is>
       </c>
       <c r="E851" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-/214748/</t>
+          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-hoforras-utca/214766/</t>
         </is>
       </c>
     </row>
     <row r="852">
-      <c r="A852" t="inlineStr">
-        <is>
-          <t>500 000</t>
-        </is>
-      </c>
-      <c r="B852" t="inlineStr">
-        <is>
-          <t>147</t>
-        </is>
-      </c>
-      <c r="C852" t="inlineStr">
-        <is>
-          <t>3 Bedrooms, 2 Bathrooms</t>
-        </is>
-      </c>
+      <c r="A852" t="inlineStr"/>
+      <c r="B852" t="inlineStr"/>
+      <c r="C852" t="inlineStr"/>
       <c r="D852" t="inlineStr">
         <is>
-          <t>Hajdúszoboszló, Hőforrás utca</t>
+          <t>Debrecen, Böszörményi út</t>
         </is>
       </c>
       <c r="E852" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-hoforras-utca/214766/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-boszormenyi-ut/212458/</t>
         </is>
       </c>
     </row>
     <row r="853">
-      <c r="A853" t="inlineStr"/>
-      <c r="B853" t="inlineStr"/>
-      <c r="C853" t="inlineStr"/>
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>420 000</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>4 Bedrooms, 2 Bathrooms</t>
+        </is>
+      </c>
       <c r="D853" t="inlineStr">
         <is>
-          <t>Debrecen, Böszörményi út</t>
+          <t>Debrecen, Simonyi út</t>
         </is>
       </c>
       <c r="E853" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-boszormenyi-ut/212458/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-simonyi-ut/212003/</t>
         </is>
       </c>
     </row>
     <row r="854">
       <c r="A854" t="inlineStr">
         <is>
-          <t>420 000</t>
+          <t>220 000</t>
         </is>
       </c>
       <c r="B854" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>71</t>
         </is>
       </c>
       <c r="C854" t="inlineStr">
         <is>
-          <t>4 Bedrooms, 2 Bathrooms</t>
+          <t>2 Bedrooms, 1 Bathrooms</t>
         </is>
       </c>
       <c r="D854" t="inlineStr">
         <is>
-          <t>Debrecen, Simonyi út</t>
+          <t>Debrecen, Böszörményi út</t>
         </is>
       </c>
       <c r="E854" t="inlineStr">
-        <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-simonyi-ut/212003/</t>
-        </is>
-      </c>
-    </row>
-    <row r="855">
-      <c r="A855" t="inlineStr">
-        <is>
-          <t>220 000</t>
-        </is>
-      </c>
-      <c r="B855" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="C855" t="inlineStr">
-        <is>
-          <t>2 Bedrooms, 1 Bathrooms</t>
-        </is>
-      </c>
-      <c r="D855" t="inlineStr">
-        <is>
-          <t>Debrecen, Böszörményi út</t>
-        </is>
-      </c>
-      <c r="E855" t="inlineStr">
         <is>
           <t>https://debrecenrent.hu/for-rent/flat/debrecen-boszormenyi-ut/209447/</t>
         </is>

</xml_diff>